<commit_message>
android back button works as pause button. add spanish translations to all scenarios
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
@@ -2695,8 +2695,8 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A142" sqref="A142"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5672,7 +5672,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="8">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="8">
         <v>5</v>

</xml_diff>

<commit_message>
remove tutorial screenshot and reuse game assets instead Localize scenario titles
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
@@ -2695,8 +2695,8 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
removal of impossible scenarios in valencia
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Valencia/AllValenciaScenarios.xlsx
@@ -1646,8 +1646,8 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3076,7 +3076,7 @@
         <v>237</v>
       </c>
       <c r="E24" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="11">
         <v>6</v>
@@ -3510,7 +3510,7 @@
         <v>249</v>
       </c>
       <c r="E31" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F31" s="11">
         <v>5</v>
@@ -3699,7 +3699,7 @@
         <v>-1</v>
       </c>
       <c r="F34" s="11">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="G34" s="11">
         <v>-1</v>
@@ -4378,7 +4378,7 @@
         <v>59</v>
       </c>
       <c r="E45" s="11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F45" s="11">
         <v>7</v>
@@ -5556,7 +5556,7 @@
         <v>89</v>
       </c>
       <c r="E64" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F64" s="11">
         <v>6</v>
@@ -6486,7 +6486,7 @@
         <v>110</v>
       </c>
       <c r="E79" s="11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F79" s="11">
         <v>4</v>
@@ -7602,7 +7602,7 @@
         <v>135</v>
       </c>
       <c r="E97" s="11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F97" s="11">
         <v>4</v>
@@ -7726,7 +7726,7 @@
         <v>328</v>
       </c>
       <c r="E99" s="11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F99" s="11">
         <v>7</v>
@@ -8036,7 +8036,7 @@
         <v>142</v>
       </c>
       <c r="E104" s="11">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F104" s="11">
         <v>4</v>
@@ -8466,7 +8466,7 @@
         <v>148</v>
       </c>
       <c r="E111" s="11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F111" s="11">
         <v>6</v>
@@ -8896,7 +8896,7 @@
         <v>159</v>
       </c>
       <c r="E118" s="11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F118" s="11">
         <v>5</v>
@@ -9330,10 +9330,10 @@
         <v>173</v>
       </c>
       <c r="E125" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F125" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G125" s="11">
         <v>-1</v>
@@ -9392,10 +9392,10 @@
         <v>174</v>
       </c>
       <c r="E126" s="11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F126" s="11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G126" s="11">
         <v>-1</v>
@@ -9454,10 +9454,10 @@
         <v>175</v>
       </c>
       <c r="E127" s="11">
+        <v>6</v>
+      </c>
+      <c r="F127" s="11">
         <v>7</v>
-      </c>
-      <c r="F127" s="11">
-        <v>-1</v>
       </c>
       <c r="G127" s="11">
         <v>-1</v>
@@ -9826,7 +9826,7 @@
         <v>369</v>
       </c>
       <c r="E133" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F133" s="11">
         <v>5</v>
@@ -10260,7 +10260,7 @@
         <v>190</v>
       </c>
       <c r="E140" s="11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F140" s="11">
         <v>5</v>

</xml_diff>